<commit_message>
se modifico el path de los archivos dentro del UDAS
</commit_message>
<xml_diff>
--- a/Media/usb1/Test_data/Udas.xlsx
+++ b/Media/usb1/Test_data/Udas.xlsx
@@ -359,7 +359,7 @@
     <t xml:space="preserve">Noche1_DanyUrrego</t>
   </si>
   <si>
-    <t xml:space="preserve">./Test_data</t>
+    <t xml:space="preserve">/Test_data</t>
   </si>
   <si>
     <t xml:space="preserve">no se conoce</t>
@@ -455,7 +455,7 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -550,17 +550,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -664,7 +653,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -805,14 +794,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -821,10 +802,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -839,10 +816,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -879,86 +852,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC0C0C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF333333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -977,7 +870,7 @@
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.89"/>
@@ -1916,8 +1809,8 @@
     <hyperlink ref="C11" r:id="rId1" display="david.lunan@udea.edu.co"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1933,10 +1826,10 @@
   <dimension ref="A1:BI31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.58"/>
@@ -1957,7 +1850,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="23.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="18.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="19.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.68"/>
@@ -1969,11 +1862,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="22.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="46" style="1" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="29.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="20.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="23.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="18.94"/>
   </cols>
   <sheetData>
@@ -2229,7 +2122,7 @@
       <c r="AB2" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AC2" s="35" t="s">
+      <c r="AC2" s="33" t="s">
         <v>121</v>
       </c>
       <c r="AD2" s="25" t="s">
@@ -2241,28 +2134,28 @@
       <c r="AF2" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="AG2" s="35" t="s">
+      <c r="AG2" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="AH2" s="35" t="s">
+      <c r="AH2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="AI2" s="36" t="s">
+      <c r="AI2" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AJ2" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="AK2" s="37" t="s">
+      <c r="AK2" s="35" t="s">
         <v>126</v>
       </c>
       <c r="AL2" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="AM2" s="35" t="s">
+      <c r="AM2" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="AN2" s="35" t="s">
+      <c r="AN2" s="33" t="s">
         <v>77</v>
       </c>
       <c r="AO2" s="34" t="s">
@@ -2280,7 +2173,7 @@
       <c r="AS2" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AT2" s="38" t="n">
+      <c r="AT2" s="36" t="n">
         <v>384000</v>
       </c>
       <c r="AU2" s="34" t="s">
@@ -2295,13 +2188,13 @@
       <c r="AX2" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="AY2" s="36" t="s">
+      <c r="AY2" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AZ2" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="BA2" s="36" t="s">
+      <c r="BA2" s="27" t="s">
         <v>120</v>
       </c>
       <c r="BB2" s="34" t="s">
@@ -2321,7 +2214,7 @@
       <c r="C3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="26" t="s">
         <v>111</v>
       </c>
       <c r="E3" s="27" t="s">
@@ -2396,7 +2289,7 @@
       <c r="AB3" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="33" t="s">
         <v>121</v>
       </c>
       <c r="AD3" s="25" t="s">
@@ -2408,28 +2301,28 @@
       <c r="AF3" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="AG3" s="35" t="s">
+      <c r="AG3" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="AH3" s="35" t="s">
+      <c r="AH3" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="AI3" s="36" t="s">
+      <c r="AI3" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AJ3" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="AK3" s="37" t="s">
+      <c r="AK3" s="35" t="s">
         <v>126</v>
       </c>
       <c r="AL3" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="AM3" s="35" t="s">
+      <c r="AM3" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="AN3" s="35" t="s">
+      <c r="AN3" s="33" t="s">
         <v>77</v>
       </c>
       <c r="AO3" s="34" t="s">
@@ -2447,7 +2340,7 @@
       <c r="AS3" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AT3" s="38" t="n">
+      <c r="AT3" s="36" t="n">
         <v>384000</v>
       </c>
       <c r="AU3" s="34" t="s">
@@ -2462,13 +2355,13 @@
       <c r="AX3" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="AY3" s="36" t="s">
+      <c r="AY3" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AZ3" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="BA3" s="36" t="s">
+      <c r="BA3" s="27" t="s">
         <v>120</v>
       </c>
       <c r="BB3" s="34" t="s">
@@ -2488,7 +2381,7 @@
       <c r="C4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="26" t="s">
         <v>111</v>
       </c>
       <c r="E4" s="27" t="s">
@@ -2536,7 +2429,7 @@
       <c r="S4" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="40" t="n">
+      <c r="T4" s="37" t="n">
         <v>1600</v>
       </c>
       <c r="U4" s="25" t="n">
@@ -2545,56 +2438,56 @@
       <c r="V4" s="25" t="n">
         <v>2021</v>
       </c>
-      <c r="W4" s="41" t="n">
+      <c r="W4" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="X4" s="42" t="n">
+      <c r="X4" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="Y4" s="35" t="n">
+      <c r="Y4" s="33" t="n">
         <v>2021</v>
       </c>
-      <c r="Z4" s="41" t="n">
+      <c r="Z4" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="AA4" s="43" t="n">
+      <c r="AA4" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35" t="s">
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="33" t="s">
         <v>135</v>
       </c>
       <c r="AD4" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="AE4" s="41" t="n">
+      <c r="AE4" s="38" t="n">
         <v>20211104</v>
       </c>
       <c r="AF4" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="AG4" s="35" t="s">
+      <c r="AG4" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="AH4" s="35" t="s">
+      <c r="AH4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="AI4" s="36" t="s">
+      <c r="AI4" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AJ4" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="AK4" s="37" t="s">
+      <c r="AK4" s="35" t="s">
         <v>126</v>
       </c>
       <c r="AL4" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="AM4" s="35" t="s">
+      <c r="AM4" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="AN4" s="35" t="s">
+      <c r="AN4" s="33" t="s">
         <v>77</v>
       </c>
       <c r="AO4" s="34" t="s">
@@ -2606,13 +2499,13 @@
       <c r="AQ4" s="25" t="n">
         <v>15</v>
       </c>
-      <c r="AR4" s="35" t="n">
+      <c r="AR4" s="33" t="n">
         <v>1</v>
       </c>
       <c r="AS4" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AT4" s="38" t="n">
+      <c r="AT4" s="36" t="n">
         <v>384000</v>
       </c>
       <c r="AU4" s="34" t="s">
@@ -2627,13 +2520,13 @@
       <c r="AX4" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="AY4" s="36" t="s">
+      <c r="AY4" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AZ4" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="BA4" s="36" t="s">
+      <c r="BA4" s="27" t="s">
         <v>120</v>
       </c>
       <c r="BB4" s="34" t="s">
@@ -2653,7 +2546,7 @@
       <c r="C5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="26" t="s">
         <v>111</v>
       </c>
       <c r="E5" s="27" t="s">
@@ -2701,7 +2594,7 @@
       <c r="S5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="T5" s="40" t="n">
+      <c r="T5" s="37" t="n">
         <v>1600</v>
       </c>
       <c r="U5" s="25" t="n">
@@ -2710,56 +2603,56 @@
       <c r="V5" s="25" t="n">
         <v>2021</v>
       </c>
-      <c r="W5" s="41" t="n">
+      <c r="W5" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="X5" s="42" t="n">
+      <c r="X5" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="Y5" s="35" t="n">
+      <c r="Y5" s="33" t="n">
         <v>2021</v>
       </c>
-      <c r="Z5" s="41" t="n">
+      <c r="Z5" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="AA5" s="43" t="n">
+      <c r="AA5" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35" t="s">
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33" t="s">
         <v>135</v>
       </c>
       <c r="AD5" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="AE5" s="41" t="n">
+      <c r="AE5" s="38" t="n">
         <v>20211104</v>
       </c>
       <c r="AF5" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="AG5" s="35" t="s">
+      <c r="AG5" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="AH5" s="35" t="s">
+      <c r="AH5" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="AI5" s="36" t="s">
+      <c r="AI5" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AJ5" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="AK5" s="37" t="s">
+      <c r="AK5" s="35" t="s">
         <v>126</v>
       </c>
       <c r="AL5" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="AM5" s="35" t="s">
+      <c r="AM5" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="AN5" s="35" t="s">
+      <c r="AN5" s="33" t="s">
         <v>77</v>
       </c>
       <c r="AO5" s="34" t="s">
@@ -2771,13 +2664,13 @@
       <c r="AQ5" s="25" t="n">
         <v>15</v>
       </c>
-      <c r="AR5" s="35" t="n">
+      <c r="AR5" s="33" t="n">
         <v>1</v>
       </c>
       <c r="AS5" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="AT5" s="38" t="n">
+      <c r="AT5" s="36" t="n">
         <v>384000</v>
       </c>
       <c r="AU5" s="34" t="s">
@@ -2792,13 +2685,13 @@
       <c r="AX5" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="AY5" s="44" t="s">
+      <c r="AY5" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AZ5" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="BA5" s="36" t="s">
+      <c r="BA5" s="27" t="s">
         <v>120</v>
       </c>
       <c r="BB5" s="34" t="s">
@@ -2823,38 +2716,38 @@
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="27"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="41"/>
-      <c r="AF6" s="35"/>
-      <c r="AG6" s="35"/>
-      <c r="AH6" s="35"/>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="45"/>
-      <c r="AL6" s="35"/>
-      <c r="AM6" s="35"/>
-      <c r="AN6" s="35"/>
-      <c r="AO6" s="35"/>
-      <c r="AP6" s="35"/>
-      <c r="AQ6" s="35"/>
-      <c r="AR6" s="35"/>
-      <c r="AS6" s="46"/>
-      <c r="AT6" s="35"/>
-      <c r="AU6" s="35"/>
-      <c r="AV6" s="41"/>
-      <c r="AW6" s="35"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="33"/>
+      <c r="AD6" s="33"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="33"/>
+      <c r="AG6" s="33"/>
+      <c r="AH6" s="33"/>
+      <c r="AI6" s="33"/>
+      <c r="AJ6" s="33"/>
+      <c r="AK6" s="41"/>
+      <c r="AL6" s="33"/>
+      <c r="AM6" s="33"/>
+      <c r="AN6" s="33"/>
+      <c r="AO6" s="33"/>
+      <c r="AP6" s="33"/>
+      <c r="AQ6" s="33"/>
+      <c r="AR6" s="33"/>
+      <c r="AS6" s="42"/>
+      <c r="AT6" s="33"/>
+      <c r="AU6" s="33"/>
+      <c r="AV6" s="38"/>
+      <c r="AW6" s="33"/>
       <c r="AX6" s="27"/>
       <c r="AY6" s="27"/>
       <c r="AZ6" s="27"/>
@@ -2877,38 +2770,38 @@
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="27"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="35"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="35"/>
-      <c r="AG7" s="35"/>
-      <c r="AH7" s="35"/>
-      <c r="AI7" s="35"/>
-      <c r="AJ7" s="35"/>
-      <c r="AK7" s="45"/>
-      <c r="AL7" s="35"/>
-      <c r="AM7" s="35"/>
-      <c r="AN7" s="35"/>
-      <c r="AO7" s="35"/>
-      <c r="AP7" s="35"/>
-      <c r="AQ7" s="35"/>
-      <c r="AR7" s="35"/>
-      <c r="AS7" s="46"/>
-      <c r="AT7" s="35"/>
-      <c r="AU7" s="35"/>
-      <c r="AV7" s="41"/>
-      <c r="AW7" s="35"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="39"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="40"/>
+      <c r="AB7" s="33"/>
+      <c r="AC7" s="33"/>
+      <c r="AD7" s="33"/>
+      <c r="AE7" s="38"/>
+      <c r="AF7" s="33"/>
+      <c r="AG7" s="33"/>
+      <c r="AH7" s="33"/>
+      <c r="AI7" s="33"/>
+      <c r="AJ7" s="33"/>
+      <c r="AK7" s="41"/>
+      <c r="AL7" s="33"/>
+      <c r="AM7" s="33"/>
+      <c r="AN7" s="33"/>
+      <c r="AO7" s="33"/>
+      <c r="AP7" s="33"/>
+      <c r="AQ7" s="33"/>
+      <c r="AR7" s="33"/>
+      <c r="AS7" s="42"/>
+      <c r="AT7" s="33"/>
+      <c r="AU7" s="33"/>
+      <c r="AV7" s="38"/>
+      <c r="AW7" s="33"/>
       <c r="AX7" s="27"/>
       <c r="AY7" s="27"/>
       <c r="AZ7" s="27"/>
@@ -2987,38 +2880,38 @@
       <c r="O9" s="31"/>
       <c r="P9" s="31"/>
       <c r="Q9" s="27"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="42"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="35"/>
-      <c r="AE9" s="41"/>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="35"/>
-      <c r="AH9" s="35"/>
-      <c r="AI9" s="35"/>
-      <c r="AJ9" s="35"/>
-      <c r="AK9" s="45"/>
-      <c r="AL9" s="35"/>
-      <c r="AM9" s="35"/>
-      <c r="AN9" s="35"/>
-      <c r="AO9" s="35"/>
-      <c r="AP9" s="35"/>
-      <c r="AQ9" s="35"/>
-      <c r="AR9" s="35"/>
-      <c r="AS9" s="46"/>
-      <c r="AT9" s="35"/>
-      <c r="AU9" s="35"/>
-      <c r="AV9" s="41"/>
-      <c r="AW9" s="35"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="33"/>
+      <c r="AD9" s="33"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="33"/>
+      <c r="AG9" s="33"/>
+      <c r="AH9" s="33"/>
+      <c r="AI9" s="33"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="41"/>
+      <c r="AL9" s="33"/>
+      <c r="AM9" s="33"/>
+      <c r="AN9" s="33"/>
+      <c r="AO9" s="33"/>
+      <c r="AP9" s="33"/>
+      <c r="AQ9" s="33"/>
+      <c r="AR9" s="33"/>
+      <c r="AS9" s="42"/>
+      <c r="AT9" s="33"/>
+      <c r="AU9" s="33"/>
+      <c r="AV9" s="38"/>
+      <c r="AW9" s="33"/>
       <c r="AX9" s="27"/>
       <c r="AY9" s="27"/>
       <c r="AZ9" s="27"/>
@@ -3041,38 +2934,38 @@
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
       <c r="Q10" s="27"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="35"/>
-      <c r="AC10" s="35"/>
-      <c r="AD10" s="35"/>
-      <c r="AE10" s="41"/>
-      <c r="AF10" s="35"/>
-      <c r="AG10" s="35"/>
-      <c r="AH10" s="35"/>
-      <c r="AI10" s="35"/>
-      <c r="AJ10" s="35"/>
-      <c r="AK10" s="45"/>
-      <c r="AL10" s="35"/>
-      <c r="AM10" s="35"/>
-      <c r="AN10" s="35"/>
-      <c r="AO10" s="35"/>
-      <c r="AP10" s="35"/>
-      <c r="AQ10" s="35"/>
-      <c r="AR10" s="35"/>
-      <c r="AS10" s="46"/>
-      <c r="AT10" s="35"/>
-      <c r="AU10" s="35"/>
-      <c r="AV10" s="41"/>
-      <c r="AW10" s="35"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="40"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="33"/>
+      <c r="AI10" s="33"/>
+      <c r="AJ10" s="33"/>
+      <c r="AK10" s="41"/>
+      <c r="AL10" s="33"/>
+      <c r="AM10" s="33"/>
+      <c r="AN10" s="33"/>
+      <c r="AO10" s="33"/>
+      <c r="AP10" s="33"/>
+      <c r="AQ10" s="33"/>
+      <c r="AR10" s="33"/>
+      <c r="AS10" s="42"/>
+      <c r="AT10" s="33"/>
+      <c r="AU10" s="33"/>
+      <c r="AV10" s="38"/>
+      <c r="AW10" s="33"/>
       <c r="AX10" s="27"/>
       <c r="AY10" s="27"/>
       <c r="AZ10" s="27"/>
@@ -3095,38 +2988,38 @@
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
       <c r="Q11" s="27"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="35"/>
-      <c r="AC11" s="35"/>
-      <c r="AD11" s="35"/>
-      <c r="AE11" s="41"/>
-      <c r="AF11" s="35"/>
-      <c r="AG11" s="35"/>
-      <c r="AH11" s="35"/>
-      <c r="AI11" s="35"/>
-      <c r="AJ11" s="35"/>
-      <c r="AK11" s="45"/>
-      <c r="AL11" s="35"/>
-      <c r="AM11" s="35"/>
-      <c r="AN11" s="35"/>
-      <c r="AO11" s="35"/>
-      <c r="AP11" s="35"/>
-      <c r="AQ11" s="35"/>
-      <c r="AR11" s="35"/>
-      <c r="AS11" s="46"/>
-      <c r="AT11" s="35"/>
-      <c r="AU11" s="35"/>
-      <c r="AV11" s="41"/>
-      <c r="AW11" s="35"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="39"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="40"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="33"/>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="33"/>
+      <c r="AG11" s="33"/>
+      <c r="AH11" s="33"/>
+      <c r="AI11" s="33"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="41"/>
+      <c r="AL11" s="33"/>
+      <c r="AM11" s="33"/>
+      <c r="AN11" s="33"/>
+      <c r="AO11" s="33"/>
+      <c r="AP11" s="33"/>
+      <c r="AQ11" s="33"/>
+      <c r="AR11" s="33"/>
+      <c r="AS11" s="42"/>
+      <c r="AT11" s="33"/>
+      <c r="AU11" s="33"/>
+      <c r="AV11" s="38"/>
+      <c r="AW11" s="33"/>
       <c r="AX11" s="27"/>
       <c r="AY11" s="27"/>
       <c r="AZ11" s="27"/>
@@ -3149,38 +3042,38 @@
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="27"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="42"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="35"/>
-      <c r="AE12" s="41"/>
-      <c r="AF12" s="35"/>
-      <c r="AG12" s="35"/>
-      <c r="AH12" s="35"/>
-      <c r="AI12" s="35"/>
-      <c r="AJ12" s="35"/>
-      <c r="AK12" s="45"/>
-      <c r="AL12" s="35"/>
-      <c r="AM12" s="35"/>
-      <c r="AN12" s="35"/>
-      <c r="AO12" s="35"/>
-      <c r="AP12" s="35"/>
-      <c r="AQ12" s="35"/>
-      <c r="AR12" s="35"/>
-      <c r="AS12" s="46"/>
-      <c r="AT12" s="35"/>
-      <c r="AU12" s="35"/>
-      <c r="AV12" s="41"/>
-      <c r="AW12" s="35"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="40"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="38"/>
+      <c r="AF12" s="33"/>
+      <c r="AG12" s="33"/>
+      <c r="AH12" s="33"/>
+      <c r="AI12" s="33"/>
+      <c r="AJ12" s="33"/>
+      <c r="AK12" s="41"/>
+      <c r="AL12" s="33"/>
+      <c r="AM12" s="33"/>
+      <c r="AN12" s="33"/>
+      <c r="AO12" s="33"/>
+      <c r="AP12" s="33"/>
+      <c r="AQ12" s="33"/>
+      <c r="AR12" s="33"/>
+      <c r="AS12" s="42"/>
+      <c r="AT12" s="33"/>
+      <c r="AU12" s="33"/>
+      <c r="AV12" s="38"/>
+      <c r="AW12" s="33"/>
       <c r="AX12" s="27"/>
       <c r="AY12" s="27"/>
       <c r="AZ12" s="27"/>
@@ -3203,38 +3096,38 @@
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
       <c r="Q13" s="27"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="42"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
-      <c r="AE13" s="41"/>
-      <c r="AF13" s="35"/>
-      <c r="AG13" s="35"/>
-      <c r="AH13" s="35"/>
-      <c r="AI13" s="35"/>
-      <c r="AJ13" s="35"/>
-      <c r="AK13" s="45"/>
-      <c r="AL13" s="35"/>
-      <c r="AM13" s="35"/>
-      <c r="AN13" s="35"/>
-      <c r="AO13" s="35"/>
-      <c r="AP13" s="35"/>
-      <c r="AQ13" s="35"/>
-      <c r="AR13" s="35"/>
-      <c r="AS13" s="46"/>
-      <c r="AT13" s="35"/>
-      <c r="AU13" s="35"/>
-      <c r="AV13" s="41"/>
-      <c r="AW13" s="35"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="40"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="33"/>
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="33"/>
+      <c r="AG13" s="33"/>
+      <c r="AH13" s="33"/>
+      <c r="AI13" s="33"/>
+      <c r="AJ13" s="33"/>
+      <c r="AK13" s="41"/>
+      <c r="AL13" s="33"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="33"/>
+      <c r="AO13" s="33"/>
+      <c r="AP13" s="33"/>
+      <c r="AQ13" s="33"/>
+      <c r="AR13" s="33"/>
+      <c r="AS13" s="42"/>
+      <c r="AT13" s="33"/>
+      <c r="AU13" s="33"/>
+      <c r="AV13" s="38"/>
+      <c r="AW13" s="33"/>
       <c r="AX13" s="27"/>
       <c r="AY13" s="27"/>
       <c r="AZ13" s="27"/>
@@ -3257,38 +3150,38 @@
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
       <c r="Q14" s="27"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="42"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="43"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
-      <c r="AE14" s="41"/>
-      <c r="AF14" s="35"/>
-      <c r="AG14" s="35"/>
-      <c r="AH14" s="35"/>
-      <c r="AI14" s="35"/>
-      <c r="AJ14" s="35"/>
-      <c r="AK14" s="45"/>
-      <c r="AL14" s="35"/>
-      <c r="AM14" s="35"/>
-      <c r="AN14" s="35"/>
-      <c r="AO14" s="35"/>
-      <c r="AP14" s="35"/>
-      <c r="AQ14" s="35"/>
-      <c r="AR14" s="35"/>
-      <c r="AS14" s="46"/>
-      <c r="AT14" s="35"/>
-      <c r="AU14" s="35"/>
-      <c r="AV14" s="41"/>
-      <c r="AW14" s="35"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="33"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="38"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="40"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="33"/>
+      <c r="AE14" s="38"/>
+      <c r="AF14" s="33"/>
+      <c r="AG14" s="33"/>
+      <c r="AH14" s="33"/>
+      <c r="AI14" s="33"/>
+      <c r="AJ14" s="33"/>
+      <c r="AK14" s="41"/>
+      <c r="AL14" s="33"/>
+      <c r="AM14" s="33"/>
+      <c r="AN14" s="33"/>
+      <c r="AO14" s="33"/>
+      <c r="AP14" s="33"/>
+      <c r="AQ14" s="33"/>
+      <c r="AR14" s="33"/>
+      <c r="AS14" s="42"/>
+      <c r="AT14" s="33"/>
+      <c r="AU14" s="33"/>
+      <c r="AV14" s="38"/>
+      <c r="AW14" s="33"/>
       <c r="AX14" s="27"/>
       <c r="AY14" s="27"/>
       <c r="AZ14" s="27"/>
@@ -3311,38 +3204,38 @@
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
       <c r="Q15" s="27"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="42"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="43"/>
-      <c r="AB15" s="35"/>
-      <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="35"/>
-      <c r="AG15" s="35"/>
-      <c r="AH15" s="35"/>
-      <c r="AI15" s="35"/>
-      <c r="AJ15" s="35"/>
-      <c r="AK15" s="45"/>
-      <c r="AL15" s="35"/>
-      <c r="AM15" s="35"/>
-      <c r="AN15" s="35"/>
-      <c r="AO15" s="35"/>
-      <c r="AP15" s="35"/>
-      <c r="AQ15" s="35"/>
-      <c r="AR15" s="35"/>
-      <c r="AS15" s="46"/>
-      <c r="AT15" s="35"/>
-      <c r="AU15" s="35"/>
-      <c r="AV15" s="41"/>
-      <c r="AW15" s="35"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="33"/>
+      <c r="T15" s="33"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="39"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="33"/>
+      <c r="AD15" s="33"/>
+      <c r="AE15" s="38"/>
+      <c r="AF15" s="33"/>
+      <c r="AG15" s="33"/>
+      <c r="AH15" s="33"/>
+      <c r="AI15" s="33"/>
+      <c r="AJ15" s="33"/>
+      <c r="AK15" s="41"/>
+      <c r="AL15" s="33"/>
+      <c r="AM15" s="33"/>
+      <c r="AN15" s="33"/>
+      <c r="AO15" s="33"/>
+      <c r="AP15" s="33"/>
+      <c r="AQ15" s="33"/>
+      <c r="AR15" s="33"/>
+      <c r="AS15" s="42"/>
+      <c r="AT15" s="33"/>
+      <c r="AU15" s="33"/>
+      <c r="AV15" s="38"/>
+      <c r="AW15" s="33"/>
       <c r="AX15" s="27"/>
       <c r="AY15" s="27"/>
       <c r="AZ15" s="27"/>
@@ -3365,38 +3258,38 @@
       <c r="O16" s="31"/>
       <c r="P16" s="31"/>
       <c r="Q16" s="27"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="41"/>
-      <c r="AA16" s="43"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
-      <c r="AE16" s="41"/>
-      <c r="AF16" s="35"/>
-      <c r="AG16" s="35"/>
-      <c r="AH16" s="35"/>
-      <c r="AI16" s="35"/>
-      <c r="AJ16" s="35"/>
-      <c r="AK16" s="45"/>
-      <c r="AL16" s="35"/>
-      <c r="AM16" s="35"/>
-      <c r="AN16" s="35"/>
-      <c r="AO16" s="35"/>
-      <c r="AP16" s="35"/>
-      <c r="AQ16" s="35"/>
-      <c r="AR16" s="35"/>
-      <c r="AS16" s="46"/>
-      <c r="AT16" s="35"/>
-      <c r="AU16" s="35"/>
-      <c r="AV16" s="41"/>
-      <c r="AW16" s="35"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
+      <c r="U16" s="33"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="38"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="40"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="33"/>
+      <c r="AE16" s="38"/>
+      <c r="AF16" s="33"/>
+      <c r="AG16" s="33"/>
+      <c r="AH16" s="33"/>
+      <c r="AI16" s="33"/>
+      <c r="AJ16" s="33"/>
+      <c r="AK16" s="41"/>
+      <c r="AL16" s="33"/>
+      <c r="AM16" s="33"/>
+      <c r="AN16" s="33"/>
+      <c r="AO16" s="33"/>
+      <c r="AP16" s="33"/>
+      <c r="AQ16" s="33"/>
+      <c r="AR16" s="33"/>
+      <c r="AS16" s="42"/>
+      <c r="AT16" s="33"/>
+      <c r="AU16" s="33"/>
+      <c r="AV16" s="38"/>
+      <c r="AW16" s="33"/>
       <c r="AX16" s="27"/>
       <c r="AY16" s="27"/>
       <c r="AZ16" s="27"/>
@@ -3419,38 +3312,38 @@
       <c r="O17" s="31"/>
       <c r="P17" s="31"/>
       <c r="Q17" s="27"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="43"/>
-      <c r="AB17" s="35"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="41"/>
-      <c r="AF17" s="35"/>
-      <c r="AG17" s="35"/>
-      <c r="AH17" s="35"/>
-      <c r="AI17" s="35"/>
-      <c r="AJ17" s="35"/>
-      <c r="AK17" s="45"/>
-      <c r="AL17" s="35"/>
-      <c r="AM17" s="35"/>
-      <c r="AN17" s="35"/>
-      <c r="AO17" s="35"/>
-      <c r="AP17" s="35"/>
-      <c r="AQ17" s="35"/>
-      <c r="AR17" s="35"/>
-      <c r="AS17" s="46"/>
-      <c r="AT17" s="35"/>
-      <c r="AU17" s="35"/>
-      <c r="AV17" s="41"/>
-      <c r="AW17" s="35"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="40"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="33"/>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="33"/>
+      <c r="AG17" s="33"/>
+      <c r="AH17" s="33"/>
+      <c r="AI17" s="33"/>
+      <c r="AJ17" s="33"/>
+      <c r="AK17" s="41"/>
+      <c r="AL17" s="33"/>
+      <c r="AM17" s="33"/>
+      <c r="AN17" s="33"/>
+      <c r="AO17" s="33"/>
+      <c r="AP17" s="33"/>
+      <c r="AQ17" s="33"/>
+      <c r="AR17" s="33"/>
+      <c r="AS17" s="42"/>
+      <c r="AT17" s="33"/>
+      <c r="AU17" s="33"/>
+      <c r="AV17" s="38"/>
+      <c r="AW17" s="33"/>
       <c r="AX17" s="27"/>
       <c r="AY17" s="27"/>
       <c r="AZ17" s="27"/>
@@ -3473,38 +3366,38 @@
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="27"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="43"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="41"/>
-      <c r="AF18" s="35"/>
-      <c r="AG18" s="35"/>
-      <c r="AH18" s="35"/>
-      <c r="AI18" s="35"/>
-      <c r="AJ18" s="35"/>
-      <c r="AK18" s="45"/>
-      <c r="AL18" s="35"/>
-      <c r="AM18" s="35"/>
-      <c r="AN18" s="35"/>
-      <c r="AO18" s="35"/>
-      <c r="AP18" s="35"/>
-      <c r="AQ18" s="35"/>
-      <c r="AR18" s="35"/>
-      <c r="AS18" s="46"/>
-      <c r="AT18" s="35"/>
-      <c r="AU18" s="35"/>
-      <c r="AV18" s="41"/>
-      <c r="AW18" s="35"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="39"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="33"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="33"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="33"/>
+      <c r="AI18" s="33"/>
+      <c r="AJ18" s="33"/>
+      <c r="AK18" s="41"/>
+      <c r="AL18" s="33"/>
+      <c r="AM18" s="33"/>
+      <c r="AN18" s="33"/>
+      <c r="AO18" s="33"/>
+      <c r="AP18" s="33"/>
+      <c r="AQ18" s="33"/>
+      <c r="AR18" s="33"/>
+      <c r="AS18" s="42"/>
+      <c r="AT18" s="33"/>
+      <c r="AU18" s="33"/>
+      <c r="AV18" s="38"/>
+      <c r="AW18" s="33"/>
       <c r="AX18" s="27"/>
       <c r="AY18" s="27"/>
       <c r="AZ18" s="27"/>
@@ -3527,41 +3420,41 @@
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
       <c r="Q19" s="27"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="47"/>
-      <c r="Y19" s="35"/>
-      <c r="Z19" s="41"/>
-      <c r="AA19" s="48"/>
-      <c r="AB19" s="35"/>
-      <c r="AC19" s="35"/>
-      <c r="AD19" s="35"/>
-      <c r="AE19" s="41"/>
-      <c r="AF19" s="35"/>
-      <c r="AG19" s="35"/>
-      <c r="AH19" s="35"/>
-      <c r="AI19" s="35"/>
-      <c r="AJ19" s="35"/>
-      <c r="AK19" s="45"/>
-      <c r="AL19" s="35"/>
-      <c r="AM19" s="35"/>
-      <c r="AN19" s="35"/>
-      <c r="AO19" s="35"/>
-      <c r="AP19" s="35"/>
-      <c r="AQ19" s="35"/>
-      <c r="AR19" s="35"/>
-      <c r="AS19" s="46"/>
-      <c r="AT19" s="35"/>
-      <c r="AU19" s="35"/>
-      <c r="AV19" s="41"/>
-      <c r="AW19" s="35"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="43"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="44"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="33"/>
+      <c r="AD19" s="33"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="33"/>
+      <c r="AG19" s="33"/>
+      <c r="AH19" s="33"/>
+      <c r="AI19" s="33"/>
+      <c r="AJ19" s="33"/>
+      <c r="AK19" s="41"/>
+      <c r="AL19" s="33"/>
+      <c r="AM19" s="33"/>
+      <c r="AN19" s="33"/>
+      <c r="AO19" s="33"/>
+      <c r="AP19" s="33"/>
+      <c r="AQ19" s="33"/>
+      <c r="AR19" s="33"/>
+      <c r="AS19" s="42"/>
+      <c r="AT19" s="33"/>
+      <c r="AU19" s="33"/>
+      <c r="AV19" s="38"/>
+      <c r="AW19" s="33"/>
       <c r="AX19" s="27"/>
       <c r="AY19" s="27"/>
-      <c r="AZ19" s="49"/>
+      <c r="AZ19" s="45"/>
       <c r="BA19" s="27"/>
       <c r="BB19" s="27"/>
       <c r="BC19" s="27"/>
@@ -3581,41 +3474,41 @@
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="27"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="35"/>
-      <c r="AC20" s="35"/>
-      <c r="AD20" s="35"/>
-      <c r="AE20" s="41"/>
-      <c r="AF20" s="35"/>
-      <c r="AG20" s="35"/>
-      <c r="AH20" s="35"/>
-      <c r="AI20" s="35"/>
-      <c r="AJ20" s="35"/>
-      <c r="AK20" s="45"/>
-      <c r="AL20" s="35"/>
-      <c r="AM20" s="35"/>
-      <c r="AN20" s="35"/>
-      <c r="AO20" s="35"/>
-      <c r="AP20" s="35"/>
-      <c r="AQ20" s="35"/>
-      <c r="AR20" s="35"/>
-      <c r="AS20" s="46"/>
-      <c r="AT20" s="35"/>
-      <c r="AU20" s="35"/>
-      <c r="AV20" s="41"/>
-      <c r="AW20" s="35"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="43"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="33"/>
+      <c r="AC20" s="33"/>
+      <c r="AD20" s="33"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="33"/>
+      <c r="AG20" s="33"/>
+      <c r="AH20" s="33"/>
+      <c r="AI20" s="33"/>
+      <c r="AJ20" s="33"/>
+      <c r="AK20" s="41"/>
+      <c r="AL20" s="33"/>
+      <c r="AM20" s="33"/>
+      <c r="AN20" s="33"/>
+      <c r="AO20" s="33"/>
+      <c r="AP20" s="33"/>
+      <c r="AQ20" s="33"/>
+      <c r="AR20" s="33"/>
+      <c r="AS20" s="42"/>
+      <c r="AT20" s="33"/>
+      <c r="AU20" s="33"/>
+      <c r="AV20" s="38"/>
+      <c r="AW20" s="33"/>
       <c r="AX20" s="27"/>
       <c r="AY20" s="27"/>
-      <c r="AZ20" s="49"/>
+      <c r="AZ20" s="45"/>
       <c r="BA20" s="27"/>
       <c r="BB20" s="27"/>
       <c r="BC20" s="27"/>
@@ -3635,41 +3528,41 @@
       <c r="O21" s="31"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="27"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="48"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="35"/>
-      <c r="AE21" s="41"/>
-      <c r="AF21" s="35"/>
-      <c r="AG21" s="35"/>
-      <c r="AH21" s="35"/>
-      <c r="AI21" s="35"/>
-      <c r="AJ21" s="35"/>
-      <c r="AK21" s="45"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="35"/>
-      <c r="AO21" s="35"/>
-      <c r="AP21" s="35"/>
-      <c r="AQ21" s="35"/>
-      <c r="AR21" s="35"/>
-      <c r="AS21" s="46"/>
-      <c r="AT21" s="35"/>
-      <c r="AU21" s="35"/>
-      <c r="AV21" s="41"/>
-      <c r="AW21" s="35"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+      <c r="T21" s="33"/>
+      <c r="U21" s="33"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="33"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="33"/>
+      <c r="AC21" s="33"/>
+      <c r="AD21" s="33"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="33"/>
+      <c r="AG21" s="33"/>
+      <c r="AH21" s="33"/>
+      <c r="AI21" s="33"/>
+      <c r="AJ21" s="33"/>
+      <c r="AK21" s="41"/>
+      <c r="AL21" s="33"/>
+      <c r="AM21" s="33"/>
+      <c r="AN21" s="33"/>
+      <c r="AO21" s="33"/>
+      <c r="AP21" s="33"/>
+      <c r="AQ21" s="33"/>
+      <c r="AR21" s="33"/>
+      <c r="AS21" s="42"/>
+      <c r="AT21" s="33"/>
+      <c r="AU21" s="33"/>
+      <c r="AV21" s="38"/>
+      <c r="AW21" s="33"/>
       <c r="AX21" s="27"/>
       <c r="AY21" s="27"/>
-      <c r="AZ21" s="49"/>
+      <c r="AZ21" s="45"/>
       <c r="BA21" s="27"/>
       <c r="BB21" s="27"/>
       <c r="BC21" s="27"/>
@@ -3689,41 +3582,41 @@
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="27"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="47"/>
-      <c r="Y22" s="35"/>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="48"/>
-      <c r="AB22" s="35"/>
-      <c r="AC22" s="35"/>
-      <c r="AD22" s="35"/>
-      <c r="AE22" s="41"/>
-      <c r="AF22" s="35"/>
-      <c r="AG22" s="35"/>
-      <c r="AH22" s="35"/>
-      <c r="AI22" s="35"/>
-      <c r="AJ22" s="35"/>
-      <c r="AK22" s="45"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
-      <c r="AN22" s="35"/>
-      <c r="AO22" s="35"/>
-      <c r="AP22" s="35"/>
-      <c r="AQ22" s="35"/>
-      <c r="AR22" s="35"/>
-      <c r="AS22" s="46"/>
-      <c r="AT22" s="35"/>
-      <c r="AU22" s="35"/>
-      <c r="AV22" s="41"/>
-      <c r="AW22" s="35"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="33"/>
+      <c r="U22" s="33"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="38"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="33"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="33"/>
+      <c r="AC22" s="33"/>
+      <c r="AD22" s="33"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="33"/>
+      <c r="AG22" s="33"/>
+      <c r="AH22" s="33"/>
+      <c r="AI22" s="33"/>
+      <c r="AJ22" s="33"/>
+      <c r="AK22" s="41"/>
+      <c r="AL22" s="33"/>
+      <c r="AM22" s="33"/>
+      <c r="AN22" s="33"/>
+      <c r="AO22" s="33"/>
+      <c r="AP22" s="33"/>
+      <c r="AQ22" s="33"/>
+      <c r="AR22" s="33"/>
+      <c r="AS22" s="42"/>
+      <c r="AT22" s="33"/>
+      <c r="AU22" s="33"/>
+      <c r="AV22" s="38"/>
+      <c r="AW22" s="33"/>
       <c r="AX22" s="27"/>
       <c r="AY22" s="27"/>
-      <c r="AZ22" s="49"/>
+      <c r="AZ22" s="45"/>
       <c r="BA22" s="27"/>
       <c r="BB22" s="27"/>
       <c r="BC22" s="27"/>
@@ -3743,41 +3636,41 @@
       <c r="O23" s="31"/>
       <c r="P23" s="31"/>
       <c r="Q23" s="27"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="47"/>
-      <c r="Y23" s="35"/>
-      <c r="Z23" s="41"/>
-      <c r="AA23" s="48"/>
-      <c r="AB23" s="35"/>
-      <c r="AC23" s="35"/>
-      <c r="AD23" s="35"/>
-      <c r="AE23" s="41"/>
-      <c r="AF23" s="35"/>
-      <c r="AG23" s="35"/>
-      <c r="AH23" s="35"/>
-      <c r="AI23" s="35"/>
-      <c r="AJ23" s="35"/>
-      <c r="AK23" s="45"/>
-      <c r="AL23" s="35"/>
-      <c r="AM23" s="35"/>
-      <c r="AN23" s="35"/>
-      <c r="AO23" s="35"/>
-      <c r="AP23" s="35"/>
-      <c r="AQ23" s="35"/>
-      <c r="AR23" s="35"/>
-      <c r="AS23" s="46"/>
-      <c r="AT23" s="35"/>
-      <c r="AU23" s="35"/>
-      <c r="AV23" s="41"/>
-      <c r="AW23" s="35"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="43"/>
+      <c r="Y23" s="33"/>
+      <c r="Z23" s="38"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="33"/>
+      <c r="AD23" s="33"/>
+      <c r="AE23" s="38"/>
+      <c r="AF23" s="33"/>
+      <c r="AG23" s="33"/>
+      <c r="AH23" s="33"/>
+      <c r="AI23" s="33"/>
+      <c r="AJ23" s="33"/>
+      <c r="AK23" s="41"/>
+      <c r="AL23" s="33"/>
+      <c r="AM23" s="33"/>
+      <c r="AN23" s="33"/>
+      <c r="AO23" s="33"/>
+      <c r="AP23" s="33"/>
+      <c r="AQ23" s="33"/>
+      <c r="AR23" s="33"/>
+      <c r="AS23" s="42"/>
+      <c r="AT23" s="33"/>
+      <c r="AU23" s="33"/>
+      <c r="AV23" s="38"/>
+      <c r="AW23" s="33"/>
       <c r="AX23" s="27"/>
       <c r="AY23" s="27"/>
-      <c r="AZ23" s="49"/>
+      <c r="AZ23" s="45"/>
       <c r="BA23" s="27"/>
       <c r="BB23" s="27"/>
       <c r="BC23" s="27"/>
@@ -3797,41 +3690,41 @@
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
       <c r="Q24" s="27"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="47"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="41"/>
-      <c r="AA24" s="48"/>
-      <c r="AB24" s="35"/>
-      <c r="AC24" s="35"/>
-      <c r="AD24" s="35"/>
-      <c r="AE24" s="41"/>
-      <c r="AF24" s="35"/>
-      <c r="AG24" s="35"/>
-      <c r="AH24" s="35"/>
-      <c r="AI24" s="35"/>
-      <c r="AJ24" s="35"/>
-      <c r="AK24" s="45"/>
-      <c r="AL24" s="35"/>
-      <c r="AM24" s="35"/>
-      <c r="AN24" s="35"/>
-      <c r="AO24" s="35"/>
-      <c r="AP24" s="35"/>
-      <c r="AQ24" s="35"/>
-      <c r="AR24" s="35"/>
-      <c r="AS24" s="46"/>
-      <c r="AT24" s="35"/>
-      <c r="AU24" s="35"/>
-      <c r="AV24" s="41"/>
-      <c r="AW24" s="35"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="38"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="33"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="44"/>
+      <c r="AB24" s="33"/>
+      <c r="AC24" s="33"/>
+      <c r="AD24" s="33"/>
+      <c r="AE24" s="38"/>
+      <c r="AF24" s="33"/>
+      <c r="AG24" s="33"/>
+      <c r="AH24" s="33"/>
+      <c r="AI24" s="33"/>
+      <c r="AJ24" s="33"/>
+      <c r="AK24" s="41"/>
+      <c r="AL24" s="33"/>
+      <c r="AM24" s="33"/>
+      <c r="AN24" s="33"/>
+      <c r="AO24" s="33"/>
+      <c r="AP24" s="33"/>
+      <c r="AQ24" s="33"/>
+      <c r="AR24" s="33"/>
+      <c r="AS24" s="42"/>
+      <c r="AT24" s="33"/>
+      <c r="AU24" s="33"/>
+      <c r="AV24" s="38"/>
+      <c r="AW24" s="33"/>
       <c r="AX24" s="27"/>
       <c r="AY24" s="27"/>
-      <c r="AZ24" s="49"/>
+      <c r="AZ24" s="45"/>
       <c r="BA24" s="27"/>
       <c r="BB24" s="27"/>
       <c r="BC24" s="27"/>
@@ -3851,41 +3744,41 @@
       <c r="O25" s="31"/>
       <c r="P25" s="31"/>
       <c r="Q25" s="27"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="47"/>
-      <c r="Y25" s="35"/>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="48"/>
-      <c r="AB25" s="35"/>
-      <c r="AC25" s="35"/>
-      <c r="AD25" s="35"/>
-      <c r="AE25" s="41"/>
-      <c r="AF25" s="35"/>
-      <c r="AG25" s="35"/>
-      <c r="AH25" s="35"/>
-      <c r="AI25" s="35"/>
-      <c r="AJ25" s="35"/>
-      <c r="AK25" s="45"/>
-      <c r="AL25" s="35"/>
-      <c r="AM25" s="35"/>
-      <c r="AN25" s="35"/>
-      <c r="AO25" s="35"/>
-      <c r="AP25" s="35"/>
-      <c r="AQ25" s="35"/>
-      <c r="AR25" s="35"/>
-      <c r="AS25" s="50"/>
-      <c r="AT25" s="35"/>
-      <c r="AU25" s="35"/>
-      <c r="AV25" s="41"/>
-      <c r="AW25" s="35"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="33"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="33"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="44"/>
+      <c r="AB25" s="33"/>
+      <c r="AC25" s="33"/>
+      <c r="AD25" s="33"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="33"/>
+      <c r="AG25" s="33"/>
+      <c r="AH25" s="33"/>
+      <c r="AI25" s="33"/>
+      <c r="AJ25" s="33"/>
+      <c r="AK25" s="41"/>
+      <c r="AL25" s="33"/>
+      <c r="AM25" s="33"/>
+      <c r="AN25" s="33"/>
+      <c r="AO25" s="33"/>
+      <c r="AP25" s="33"/>
+      <c r="AQ25" s="33"/>
+      <c r="AR25" s="33"/>
+      <c r="AS25" s="46"/>
+      <c r="AT25" s="33"/>
+      <c r="AU25" s="33"/>
+      <c r="AV25" s="38"/>
+      <c r="AW25" s="33"/>
       <c r="AX25" s="27"/>
       <c r="AY25" s="27"/>
-      <c r="AZ25" s="49"/>
+      <c r="AZ25" s="45"/>
       <c r="BA25" s="27"/>
       <c r="BB25" s="27"/>
       <c r="BC25" s="27"/>
@@ -3905,41 +3798,41 @@
       <c r="O26" s="31"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="27"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="47"/>
-      <c r="Y26" s="35"/>
-      <c r="Z26" s="41"/>
-      <c r="AA26" s="48"/>
-      <c r="AB26" s="35"/>
-      <c r="AC26" s="35"/>
-      <c r="AD26" s="35"/>
-      <c r="AE26" s="41"/>
-      <c r="AF26" s="35"/>
-      <c r="AG26" s="35"/>
-      <c r="AH26" s="35"/>
-      <c r="AI26" s="35"/>
-      <c r="AJ26" s="35"/>
-      <c r="AK26" s="45"/>
-      <c r="AL26" s="35"/>
-      <c r="AM26" s="35"/>
-      <c r="AN26" s="35"/>
-      <c r="AO26" s="35"/>
-      <c r="AP26" s="35"/>
-      <c r="AQ26" s="35"/>
-      <c r="AR26" s="35"/>
-      <c r="AS26" s="46"/>
-      <c r="AT26" s="35"/>
-      <c r="AU26" s="35"/>
-      <c r="AV26" s="41"/>
-      <c r="AW26" s="35"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="33"/>
+      <c r="T26" s="33"/>
+      <c r="U26" s="33"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="33"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="44"/>
+      <c r="AB26" s="33"/>
+      <c r="AC26" s="33"/>
+      <c r="AD26" s="33"/>
+      <c r="AE26" s="38"/>
+      <c r="AF26" s="33"/>
+      <c r="AG26" s="33"/>
+      <c r="AH26" s="33"/>
+      <c r="AI26" s="33"/>
+      <c r="AJ26" s="33"/>
+      <c r="AK26" s="41"/>
+      <c r="AL26" s="33"/>
+      <c r="AM26" s="33"/>
+      <c r="AN26" s="33"/>
+      <c r="AO26" s="33"/>
+      <c r="AP26" s="33"/>
+      <c r="AQ26" s="33"/>
+      <c r="AR26" s="33"/>
+      <c r="AS26" s="42"/>
+      <c r="AT26" s="33"/>
+      <c r="AU26" s="33"/>
+      <c r="AV26" s="38"/>
+      <c r="AW26" s="33"/>
       <c r="AX26" s="27"/>
       <c r="AY26" s="27"/>
-      <c r="AZ26" s="49"/>
+      <c r="AZ26" s="45"/>
       <c r="BA26" s="27"/>
       <c r="BB26" s="27"/>
       <c r="BC26" s="27"/>
@@ -3959,41 +3852,41 @@
       <c r="O27" s="31"/>
       <c r="P27" s="31"/>
       <c r="Q27" s="27"/>
-      <c r="R27" s="35"/>
-      <c r="S27" s="35"/>
-      <c r="T27" s="35"/>
-      <c r="U27" s="35"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="47"/>
-      <c r="Y27" s="35"/>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="48"/>
-      <c r="AB27" s="35"/>
-      <c r="AC27" s="35"/>
-      <c r="AD27" s="35"/>
-      <c r="AE27" s="41"/>
-      <c r="AF27" s="35"/>
-      <c r="AG27" s="35"/>
-      <c r="AH27" s="35"/>
-      <c r="AI27" s="35"/>
-      <c r="AJ27" s="35"/>
-      <c r="AK27" s="45"/>
-      <c r="AL27" s="35"/>
-      <c r="AM27" s="35"/>
-      <c r="AN27" s="35"/>
-      <c r="AO27" s="35"/>
-      <c r="AP27" s="35"/>
-      <c r="AQ27" s="35"/>
-      <c r="AR27" s="35"/>
-      <c r="AS27" s="46"/>
-      <c r="AT27" s="35"/>
-      <c r="AU27" s="35"/>
-      <c r="AV27" s="41"/>
-      <c r="AW27" s="35"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="33"/>
+      <c r="U27" s="33"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="43"/>
+      <c r="Y27" s="33"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="44"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="33"/>
+      <c r="AD27" s="33"/>
+      <c r="AE27" s="38"/>
+      <c r="AF27" s="33"/>
+      <c r="AG27" s="33"/>
+      <c r="AH27" s="33"/>
+      <c r="AI27" s="33"/>
+      <c r="AJ27" s="33"/>
+      <c r="AK27" s="41"/>
+      <c r="AL27" s="33"/>
+      <c r="AM27" s="33"/>
+      <c r="AN27" s="33"/>
+      <c r="AO27" s="33"/>
+      <c r="AP27" s="33"/>
+      <c r="AQ27" s="33"/>
+      <c r="AR27" s="33"/>
+      <c r="AS27" s="42"/>
+      <c r="AT27" s="33"/>
+      <c r="AU27" s="33"/>
+      <c r="AV27" s="38"/>
+      <c r="AW27" s="33"/>
       <c r="AX27" s="27"/>
       <c r="AY27" s="27"/>
-      <c r="AZ27" s="49"/>
+      <c r="AZ27" s="45"/>
       <c r="BA27" s="27"/>
       <c r="BB27" s="27"/>
       <c r="BC27" s="27"/>
@@ -4013,41 +3906,41 @@
       <c r="O28" s="31"/>
       <c r="P28" s="31"/>
       <c r="Q28" s="27"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="47"/>
-      <c r="Y28" s="35"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="48"/>
-      <c r="AB28" s="35"/>
-      <c r="AC28" s="35"/>
-      <c r="AD28" s="35"/>
-      <c r="AE28" s="41"/>
-      <c r="AF28" s="35"/>
-      <c r="AG28" s="35"/>
-      <c r="AH28" s="35"/>
-      <c r="AI28" s="35"/>
-      <c r="AJ28" s="35"/>
-      <c r="AK28" s="45"/>
-      <c r="AL28" s="35"/>
-      <c r="AM28" s="35"/>
-      <c r="AN28" s="35"/>
-      <c r="AO28" s="35"/>
-      <c r="AP28" s="35"/>
-      <c r="AQ28" s="35"/>
-      <c r="AR28" s="35"/>
-      <c r="AS28" s="46"/>
-      <c r="AT28" s="35"/>
-      <c r="AU28" s="35"/>
-      <c r="AV28" s="41"/>
-      <c r="AW28" s="35"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="38"/>
+      <c r="X28" s="43"/>
+      <c r="Y28" s="33"/>
+      <c r="Z28" s="38"/>
+      <c r="AA28" s="44"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="33"/>
+      <c r="AD28" s="33"/>
+      <c r="AE28" s="38"/>
+      <c r="AF28" s="33"/>
+      <c r="AG28" s="33"/>
+      <c r="AH28" s="33"/>
+      <c r="AI28" s="33"/>
+      <c r="AJ28" s="33"/>
+      <c r="AK28" s="41"/>
+      <c r="AL28" s="33"/>
+      <c r="AM28" s="33"/>
+      <c r="AN28" s="33"/>
+      <c r="AO28" s="33"/>
+      <c r="AP28" s="33"/>
+      <c r="AQ28" s="33"/>
+      <c r="AR28" s="33"/>
+      <c r="AS28" s="42"/>
+      <c r="AT28" s="33"/>
+      <c r="AU28" s="33"/>
+      <c r="AV28" s="38"/>
+      <c r="AW28" s="33"/>
       <c r="AX28" s="27"/>
       <c r="AY28" s="27"/>
-      <c r="AZ28" s="49"/>
+      <c r="AZ28" s="45"/>
       <c r="BA28" s="27"/>
       <c r="BB28" s="27"/>
       <c r="BC28" s="27"/>
@@ -4067,41 +3960,41 @@
       <c r="O29" s="31"/>
       <c r="P29" s="31"/>
       <c r="Q29" s="27"/>
-      <c r="R29" s="35"/>
-      <c r="S29" s="35"/>
-      <c r="T29" s="35"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="47"/>
-      <c r="Y29" s="35"/>
-      <c r="Z29" s="41"/>
-      <c r="AA29" s="48"/>
-      <c r="AB29" s="35"/>
-      <c r="AC29" s="35"/>
-      <c r="AD29" s="35"/>
-      <c r="AE29" s="41"/>
-      <c r="AF29" s="35"/>
-      <c r="AG29" s="35"/>
-      <c r="AH29" s="35"/>
-      <c r="AI29" s="35"/>
-      <c r="AJ29" s="35"/>
-      <c r="AK29" s="45"/>
-      <c r="AL29" s="35"/>
-      <c r="AM29" s="35"/>
-      <c r="AN29" s="35"/>
-      <c r="AO29" s="35"/>
-      <c r="AP29" s="35"/>
-      <c r="AQ29" s="35"/>
-      <c r="AR29" s="35"/>
-      <c r="AS29" s="46"/>
-      <c r="AT29" s="35"/>
-      <c r="AU29" s="35"/>
-      <c r="AV29" s="41"/>
-      <c r="AW29" s="35"/>
+      <c r="R29" s="33"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="33"/>
+      <c r="U29" s="33"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="38"/>
+      <c r="X29" s="43"/>
+      <c r="Y29" s="33"/>
+      <c r="Z29" s="38"/>
+      <c r="AA29" s="44"/>
+      <c r="AB29" s="33"/>
+      <c r="AC29" s="33"/>
+      <c r="AD29" s="33"/>
+      <c r="AE29" s="38"/>
+      <c r="AF29" s="33"/>
+      <c r="AG29" s="33"/>
+      <c r="AH29" s="33"/>
+      <c r="AI29" s="33"/>
+      <c r="AJ29" s="33"/>
+      <c r="AK29" s="41"/>
+      <c r="AL29" s="33"/>
+      <c r="AM29" s="33"/>
+      <c r="AN29" s="33"/>
+      <c r="AO29" s="33"/>
+      <c r="AP29" s="33"/>
+      <c r="AQ29" s="33"/>
+      <c r="AR29" s="33"/>
+      <c r="AS29" s="42"/>
+      <c r="AT29" s="33"/>
+      <c r="AU29" s="33"/>
+      <c r="AV29" s="38"/>
+      <c r="AW29" s="33"/>
       <c r="AX29" s="27"/>
       <c r="AY29" s="27"/>
-      <c r="AZ29" s="49"/>
+      <c r="AZ29" s="45"/>
       <c r="BA29" s="27"/>
       <c r="BB29" s="27"/>
       <c r="BC29" s="27"/>
@@ -4121,41 +4014,41 @@
       <c r="O30" s="31"/>
       <c r="P30" s="31"/>
       <c r="Q30" s="27"/>
-      <c r="R30" s="35"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="47"/>
-      <c r="Y30" s="35"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="48"/>
-      <c r="AB30" s="35"/>
-      <c r="AC30" s="35"/>
-      <c r="AD30" s="35"/>
-      <c r="AE30" s="41"/>
-      <c r="AF30" s="35"/>
-      <c r="AG30" s="35"/>
-      <c r="AH30" s="35"/>
-      <c r="AI30" s="35"/>
-      <c r="AJ30" s="35"/>
-      <c r="AK30" s="45"/>
-      <c r="AL30" s="35"/>
-      <c r="AM30" s="35"/>
-      <c r="AN30" s="35"/>
-      <c r="AO30" s="35"/>
-      <c r="AP30" s="35"/>
-      <c r="AQ30" s="35"/>
-      <c r="AR30" s="35"/>
-      <c r="AS30" s="46"/>
-      <c r="AT30" s="35"/>
-      <c r="AU30" s="35"/>
-      <c r="AV30" s="41"/>
-      <c r="AW30" s="35"/>
+      <c r="R30" s="33"/>
+      <c r="S30" s="33"/>
+      <c r="T30" s="33"/>
+      <c r="U30" s="33"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="38"/>
+      <c r="X30" s="43"/>
+      <c r="Y30" s="33"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30" s="44"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="33"/>
+      <c r="AD30" s="33"/>
+      <c r="AE30" s="38"/>
+      <c r="AF30" s="33"/>
+      <c r="AG30" s="33"/>
+      <c r="AH30" s="33"/>
+      <c r="AI30" s="33"/>
+      <c r="AJ30" s="33"/>
+      <c r="AK30" s="41"/>
+      <c r="AL30" s="33"/>
+      <c r="AM30" s="33"/>
+      <c r="AN30" s="33"/>
+      <c r="AO30" s="33"/>
+      <c r="AP30" s="33"/>
+      <c r="AQ30" s="33"/>
+      <c r="AR30" s="33"/>
+      <c r="AS30" s="42"/>
+      <c r="AT30" s="33"/>
+      <c r="AU30" s="33"/>
+      <c r="AV30" s="38"/>
+      <c r="AW30" s="33"/>
       <c r="AX30" s="27"/>
       <c r="AY30" s="27"/>
-      <c r="AZ30" s="49"/>
+      <c r="AZ30" s="45"/>
       <c r="BA30" s="27"/>
       <c r="BB30" s="27"/>
       <c r="BC30" s="27"/>
@@ -4175,41 +4068,41 @@
       <c r="O31" s="31"/>
       <c r="P31" s="31"/>
       <c r="Q31" s="27"/>
-      <c r="R31" s="35"/>
-      <c r="S31" s="35"/>
-      <c r="T31" s="35"/>
-      <c r="U31" s="35"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="47"/>
-      <c r="Y31" s="35"/>
-      <c r="Z31" s="41"/>
-      <c r="AA31" s="48"/>
-      <c r="AB31" s="35"/>
-      <c r="AC31" s="35"/>
-      <c r="AD31" s="35"/>
-      <c r="AE31" s="41"/>
-      <c r="AF31" s="35"/>
-      <c r="AG31" s="35"/>
-      <c r="AH31" s="35"/>
-      <c r="AI31" s="35"/>
-      <c r="AJ31" s="35"/>
-      <c r="AK31" s="45"/>
-      <c r="AL31" s="35"/>
-      <c r="AM31" s="35"/>
-      <c r="AN31" s="35"/>
-      <c r="AO31" s="35"/>
-      <c r="AP31" s="35"/>
-      <c r="AQ31" s="35"/>
-      <c r="AR31" s="35"/>
-      <c r="AS31" s="46"/>
-      <c r="AT31" s="35"/>
-      <c r="AU31" s="35"/>
-      <c r="AV31" s="41"/>
-      <c r="AW31" s="35"/>
+      <c r="R31" s="33"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="33"/>
+      <c r="U31" s="33"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="38"/>
+      <c r="X31" s="43"/>
+      <c r="Y31" s="33"/>
+      <c r="Z31" s="38"/>
+      <c r="AA31" s="44"/>
+      <c r="AB31" s="33"/>
+      <c r="AC31" s="33"/>
+      <c r="AD31" s="33"/>
+      <c r="AE31" s="38"/>
+      <c r="AF31" s="33"/>
+      <c r="AG31" s="33"/>
+      <c r="AH31" s="33"/>
+      <c r="AI31" s="33"/>
+      <c r="AJ31" s="33"/>
+      <c r="AK31" s="41"/>
+      <c r="AL31" s="33"/>
+      <c r="AM31" s="33"/>
+      <c r="AN31" s="33"/>
+      <c r="AO31" s="33"/>
+      <c r="AP31" s="33"/>
+      <c r="AQ31" s="33"/>
+      <c r="AR31" s="33"/>
+      <c r="AS31" s="42"/>
+      <c r="AT31" s="33"/>
+      <c r="AU31" s="33"/>
+      <c r="AV31" s="38"/>
+      <c r="AW31" s="33"/>
       <c r="AX31" s="27"/>
       <c r="AY31" s="27"/>
-      <c r="AZ31" s="49"/>
+      <c r="AZ31" s="45"/>
       <c r="BA31" s="27"/>
       <c r="BB31" s="27"/>
       <c r="BC31" s="27"/>
@@ -4223,8 +4116,8 @@
     <hyperlink ref="G5" r:id="rId4" display="dany.urrego@udea.edu.co"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>